<commit_message>
latest update from Imtiaz
</commit_message>
<xml_diff>
--- a/KatalonData/MultibillTestData/MultibillCCData.xlsx
+++ b/KatalonData/MultibillTestData/MultibillCCData.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="226">
   <si>
     <t>Result</t>
   </si>
@@ -719,6 +719,9 @@
   </si>
   <si>
     <t>Wed Apr 02 15:08:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Apr 08 15:12:35 EDT 2025</t>
   </si>
 </sst>
 </file>
@@ -2973,7 +2976,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">

</xml_diff>

<commit_message>
Updated and Added Test Cases for Multibill
</commit_message>
<xml_diff>
--- a/KatalonData/MultibillTestData/MultibillCCData.xlsx
+++ b/KatalonData/MultibillTestData/MultibillCCData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t465179\Documents\git\VPS-Katalon\VPS-Katalon\KatalonData\MultibillTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{95CC317F-2C51-484B-85EA-34E60EBBBEA3}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{2BC165B1-800F-460B-A2DC-993864F6B38A}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="9" firstSheet="6" windowHeight="15675" windowWidth="28995" xWindow="14303" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-2010"/>
+    <workbookView activeTab="10" firstSheet="6" windowHeight="15675" windowWidth="28995" xWindow="14303" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-2010"/>
   </bookViews>
   <sheets>
     <sheet name="CCData" r:id="rId1" sheetId="1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="158">
   <si>
     <t>Result</t>
   </si>
@@ -400,15 +400,6 @@
     <t>$*.51</t>
   </si>
   <si>
-    <t>Thu May 22 11:21:06 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Sep 17 23:53:34 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Sep 17 23:54:19 IST 2025</t>
-  </si>
-  <si>
     <t>Wed Sep 17 23:54:51 IST 2025</t>
   </si>
   <si>
@@ -418,9 +409,6 @@
     <t>Wed Sep 17 23:56:17 IST 2025</t>
   </si>
   <si>
-    <t>Thu Sep 18 00:00:31 IST 2025</t>
-  </si>
-  <si>
     <t>Thu Sep 18 00:02:05 IST 2025</t>
   </si>
   <si>
@@ -433,18 +421,6 @@
     <t>Thu Sep 18 00:06:50 IST 2025</t>
   </si>
   <si>
-    <t>Thu Sep 18 00:07:33 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Sep 18 00:08:17 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Sep 18 00:08:59 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Nov 20 18:16:17 EST 2025</t>
-  </si>
-  <si>
     <t>Thu Nov 20 19:08:46 EST 2025</t>
   </si>
   <si>
@@ -457,22 +433,91 @@
     <t>sm</t>
   </si>
   <si>
+    <t>Thu Nov 20 21:03:01 EST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 21:04:56 EST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 21:13:34 EST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 21:17:09 EST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 21:17:44 EST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 13:46:58 EST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 19:53:20 EST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 20:20:19 EST 2025</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Thu Nov 20 21:03:01 EST 2025</t>
-  </si>
-  <si>
-    <t>Thu Nov 20 21:04:56 EST 2025</t>
-  </si>
-  <si>
-    <t>Thu Nov 20 21:13:34 EST 2025</t>
-  </si>
-  <si>
-    <t>Thu Nov 20 21:17:09 EST 2025</t>
-  </si>
-  <si>
-    <t>Thu Nov 20 21:17:44 EST 2025</t>
+    <t>Mon Nov 24 14:32:13 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 24 14:36:07 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 24 14:37:36 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 24 14:40:13 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 24 14:42:23 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 24 14:44:23 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 24 14:47:01 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 24 14:52:02 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 24 15:00:14 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 24 15:02:44 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 24 15:14:07 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 24 15:18:20 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 24 15:23:58 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 24 16:00:26 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 24 16:27:57 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 24 16:30:33 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 24 16:35:36 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 24 16:40:18 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 24 16:40:54 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 24 16:42:59 EST 2025</t>
   </si>
 </sst>
 </file>
@@ -1072,7 +1117,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A8BF27D-9E5B-43D3-A8C6-55BD0B2E602C}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -1106,7 +1151,7 @@
         <v>26</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1118,8 +1163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71D7CF63-52CE-45A5-AAAD-49E5406A5D05}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1162,10 +1207,10 @@
     </row>
     <row ht="43.5" r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
@@ -1271,7 +1316,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>143</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
@@ -1333,7 +1378,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
@@ -1348,7 +1393,7 @@
         <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="D3" t="s">
         <v>26</v>
@@ -1409,7 +1454,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
@@ -1515,7 +1560,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
+        <v>144</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
@@ -1594,10 +1639,10 @@
     </row>
     <row ht="29" r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
@@ -1681,7 +1726,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
@@ -1769,10 +1814,10 @@
     </row>
     <row ht="29" r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
@@ -1860,10 +1905,10 @@
     </row>
     <row ht="29" r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>126</v>
+        <v>149</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
@@ -1961,7 +2006,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>154</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
@@ -2064,10 +2109,10 @@
     </row>
     <row ht="29" r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
@@ -2161,7 +2206,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
@@ -2250,7 +2295,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
@@ -2335,7 +2380,7 @@
         <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
@@ -2424,7 +2469,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
@@ -2648,7 +2693,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>140</v>
+        <v>157</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
@@ -2728,7 +2773,7 @@
         <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">

</xml_diff>